<commit_message>
Updatedexisting visualizations, added additional version of same.
</commit_message>
<xml_diff>
--- a/Tableau/Portland Mayoral 2019.xlsx
+++ b/Tableau/Portland Mayoral 2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_a_p\source\repos\campaign-finance\Tableau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A89B4A-88C7-4C7F-B6BF-B7496324EE16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D4D2D-FCA1-4368-8530-AE57717D7E24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{C74820B7-79AB-43DA-AF4F-6D0FFBE61A94}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C74820B7-79AB-43DA-AF4F-6D0FFBE61A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Portland Mayoral 2019" sheetId="1" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
     <t>Region</t>
   </si>
   <si>
-    <t>"From Away"</t>
+    <t>Out of State</t>
   </si>
 </sst>
 </file>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BAF182-B7C3-474F-8EBC-E513D813BF36}">
   <dimension ref="A1:L691"/>
   <sheetViews>
-    <sheetView topLeftCell="A344" workbookViewId="0">
-      <selection activeCell="L294" sqref="L193:L294"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="L379" sqref="L379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27975,8 +27975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6626CD0E-E6C8-4AD6-9BFB-8D91496D4EC8}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A1:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>